<commit_message>
tutorial and assignment 1 done. key in progress
</commit_message>
<xml_diff>
--- a/data/MMI_HW_data.xlsx
+++ b/data/MMI_HW_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_folder\R_projects_local\ENVS337\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223C66AC-38A9-4E93-95ED-C9CCC4440289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843EB7DC-9D38-4008-8837-621ED909A4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A75CC" sheetId="2" r:id="rId1"/>
-    <sheet name="taxa_info" sheetId="6" r:id="rId2"/>
-    <sheet name="other_sites" sheetId="4" r:id="rId3"/>
-    <sheet name="site_info" sheetId="8" r:id="rId4"/>
+    <sheet name="A72" sheetId="9" r:id="rId2"/>
+    <sheet name="taxa_info" sheetId="6" r:id="rId3"/>
+    <sheet name="other_sites" sheetId="4" r:id="rId4"/>
+    <sheet name="site_info" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="168">
   <si>
     <t>Class</t>
   </si>
@@ -595,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -615,10 +616,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,17 +899,17 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
@@ -923,7 +920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
@@ -934,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
@@ -945,7 +942,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -956,7 +953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -967,7 +964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -978,7 +975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>122</v>
       </c>
@@ -989,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -1011,7 +1008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>122</v>
       </c>
@@ -1022,7 +1019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>122</v>
       </c>
@@ -1044,7 +1041,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>122</v>
       </c>
@@ -1055,7 +1052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>122</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>122</v>
       </c>
@@ -1077,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>122</v>
       </c>
@@ -1088,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>122</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -1110,7 +1107,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
@@ -1121,7 +1118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>122</v>
       </c>
@@ -1132,7 +1129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>122</v>
       </c>
@@ -1143,7 +1140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
@@ -1154,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -1165,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>122</v>
       </c>
@@ -1176,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -1187,7 +1184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -1198,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>122</v>
       </c>
@@ -1220,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>122</v>
       </c>
@@ -1231,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>122</v>
       </c>
@@ -1242,7 +1239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>122</v>
       </c>
@@ -1264,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>122</v>
       </c>
@@ -1275,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
@@ -1297,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>122</v>
       </c>
@@ -1308,7 +1305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>122</v>
       </c>
@@ -1319,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>122</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>122</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>122</v>
       </c>
@@ -1374,7 +1371,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -1385,7 +1382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>122</v>
       </c>
@@ -1396,7 +1393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>122</v>
       </c>
@@ -1413,28 +1410,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB002BF-9427-4F54-99EB-0A769A51BC2F}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1466,7 +1621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
@@ -1498,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -1528,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>97</v>
       </c>
@@ -1560,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
@@ -1592,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
@@ -1624,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1656,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>159</v>
       </c>
@@ -1688,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>51</v>
       </c>
@@ -1720,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>158</v>
       </c>
@@ -1752,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>164</v>
       </c>
@@ -1784,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>52</v>
       </c>
@@ -1816,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>53</v>
       </c>
@@ -1848,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -1880,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
@@ -1912,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
@@ -1944,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>57</v>
       </c>
@@ -1976,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>58</v>
       </c>
@@ -2008,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>91</v>
       </c>
@@ -2040,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>166</v>
       </c>
@@ -2072,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
@@ -2104,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>88</v>
       </c>
@@ -2136,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -2168,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>85</v>
       </c>
@@ -2200,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>90</v>
       </c>
@@ -2232,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
@@ -2262,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
@@ -2294,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
@@ -2326,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>63</v>
       </c>
@@ -2358,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -2388,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -2420,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>86</v>
       </c>
@@ -2452,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>64</v>
       </c>
@@ -2482,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>67</v>
       </c>
@@ -2514,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>68</v>
       </c>
@@ -2546,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>66</v>
       </c>
@@ -2576,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
@@ -2608,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>10</v>
       </c>
@@ -2640,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>118</v>
       </c>
@@ -2672,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>12</v>
       </c>
@@ -2704,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>155</v>
       </c>
@@ -2736,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
@@ -2768,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>14</v>
       </c>
@@ -2800,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -2832,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>17</v>
       </c>
@@ -2864,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -2896,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>93</v>
       </c>
@@ -2958,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>100</v>
       </c>
@@ -2990,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -3022,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>156</v>
       </c>
@@ -3054,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>22</v>
       </c>
@@ -3084,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
@@ -3116,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -3148,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>25</v>
       </c>
@@ -3208,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>27</v>
       </c>
@@ -3240,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>29</v>
       </c>
@@ -3272,7 +3427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>30</v>
       </c>
@@ -3304,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>80</v>
       </c>
@@ -3336,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>28</v>
       </c>
@@ -3366,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>95</v>
       </c>
@@ -3398,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>32</v>
       </c>
@@ -3430,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>35</v>
       </c>
@@ -3462,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>87</v>
       </c>
@@ -3488,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>37</v>
       </c>
@@ -3514,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>149</v>
       </c>
@@ -3540,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>38</v>
       </c>
@@ -3566,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>36</v>
       </c>
@@ -3596,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>82</v>
       </c>
@@ -3628,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>165</v>
       </c>
@@ -3654,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>130</v>
       </c>
@@ -3680,7 +3835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>119</v>
       </c>
@@ -3712,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>163</v>
       </c>
@@ -3744,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>83</v>
       </c>
@@ -3776,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>157</v>
       </c>
@@ -3808,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>84</v>
       </c>
@@ -3840,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>152</v>
       </c>
@@ -3872,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>40</v>
       </c>
@@ -3904,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>102</v>
       </c>
@@ -3936,7 +4091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>154</v>
       </c>
@@ -3968,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>72</v>
       </c>
@@ -4000,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>74</v>
       </c>
@@ -4032,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>104</v>
       </c>
@@ -4064,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>78</v>
       </c>
@@ -4088,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>75</v>
       </c>
@@ -4114,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>76</v>
       </c>
@@ -4140,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>77</v>
       </c>
@@ -4166,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>162</v>
       </c>
@@ -4208,20 +4363,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:C142"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -4232,1554 +4387,1422 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="7">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="C9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="7">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="C14">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C15">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C21">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C23">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>134</v>
       </c>
       <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
         <v>84</v>
       </c>
-      <c r="C27">
+      <c r="C37">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
         <v>48</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C40">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C41">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
       <c r="C42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>135</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="C47">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C48">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>17</v>
       </c>
       <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>135</v>
-      </c>
-      <c r="B52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="C53">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>136</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="C58">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>136</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>136</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C60">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>158</v>
       </c>
       <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>136</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="C62">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>136</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="C63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>136</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="C64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>136</v>
       </c>
       <c r="B65" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>136</v>
       </c>
       <c r="B66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
         <v>79</v>
       </c>
-      <c r="C66">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>136</v>
-      </c>
-      <c r="B67" t="s">
-        <v>80</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>136</v>
-      </c>
-      <c r="B69" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>136</v>
-      </c>
-      <c r="B70" t="s">
-        <v>157</v>
-      </c>
       <c r="C70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C72">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>37</v>
       </c>
       <c r="C73">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C75">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B76" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="C76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>89</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>138</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>138</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C80">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>138</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C82">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C83">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>138</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>138</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C85">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C87">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" t="s">
+        <v>156</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" t="s">
+        <v>79</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" t="s">
         <v>46</v>
       </c>
-      <c r="C88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>138</v>
-      </c>
-      <c r="B89" t="s">
-        <v>48</v>
-      </c>
-      <c r="C89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>138</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>88</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>139</v>
+      </c>
+      <c r="B97" t="s">
         <v>89</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>138</v>
-      </c>
-      <c r="B91" t="s">
-        <v>50</v>
-      </c>
-      <c r="C91">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>138</v>
-      </c>
-      <c r="B92" t="s">
-        <v>52</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>138</v>
-      </c>
-      <c r="B93" t="s">
-        <v>55</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>138</v>
-      </c>
-      <c r="B94" t="s">
-        <v>86</v>
-      </c>
-      <c r="C94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>138</v>
-      </c>
-      <c r="B95" t="s">
-        <v>72</v>
-      </c>
-      <c r="C95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>138</v>
-      </c>
-      <c r="B96" t="s">
-        <v>74</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>138</v>
-      </c>
-      <c r="B97" t="s">
-        <v>77</v>
-      </c>
       <c r="C97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>139</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>139</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="C99">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>139</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C100">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>139</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>139</v>
       </c>
       <c r="B102" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>139</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C103">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>139</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="C104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>140</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>140</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>140</v>
+      </c>
+      <c r="B107" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>140</v>
+      </c>
+      <c r="B108" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>140</v>
+      </c>
+      <c r="B109" t="s">
+        <v>79</v>
+      </c>
+      <c r="C109">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>140</v>
+      </c>
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>140</v>
+      </c>
+      <c r="B111" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" t="s">
+        <v>28</v>
+      </c>
+      <c r="C112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>140</v>
+      </c>
+      <c r="B113" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>140</v>
+      </c>
+      <c r="B114" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>139</v>
-      </c>
-      <c r="B105" t="s">
-        <v>32</v>
-      </c>
-      <c r="C105">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>139</v>
-      </c>
-      <c r="B106" t="s">
-        <v>37</v>
-      </c>
-      <c r="C106">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>139</v>
-      </c>
-      <c r="B107" t="s">
-        <v>46</v>
-      </c>
-      <c r="C107">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>140</v>
+      </c>
+      <c r="B115" t="s">
+        <v>165</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>140</v>
+      </c>
+      <c r="B116" t="s">
+        <v>83</v>
+      </c>
+      <c r="C116">
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>139</v>
-      </c>
-      <c r="B108" t="s">
-        <v>88</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>139</v>
-      </c>
-      <c r="B109" t="s">
-        <v>89</v>
-      </c>
-      <c r="C109">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>139</v>
-      </c>
-      <c r="B110" t="s">
-        <v>50</v>
-      </c>
-      <c r="C110">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>139</v>
-      </c>
-      <c r="B111" t="s">
-        <v>164</v>
-      </c>
-      <c r="C111">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>139</v>
-      </c>
-      <c r="B112" t="s">
-        <v>53</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>139</v>
-      </c>
-      <c r="B113" t="s">
-        <v>62</v>
-      </c>
-      <c r="C113">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>139</v>
-      </c>
-      <c r="B114" t="s">
-        <v>86</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>139</v>
-      </c>
-      <c r="B115" t="s">
-        <v>72</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>139</v>
-      </c>
-      <c r="B116" t="s">
-        <v>74</v>
-      </c>
-      <c r="C116">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>140</v>
       </c>
       <c r="B117" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="C117">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>140</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C118">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>140</v>
       </c>
       <c r="B119" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="C119">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>140</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="C120">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>140</v>
       </c>
       <c r="B121" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C121">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>140</v>
       </c>
       <c r="B122" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>140</v>
       </c>
       <c r="B123" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>140</v>
       </c>
       <c r="B124" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C124">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C125">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>140</v>
       </c>
       <c r="B126" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="C126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>140</v>
       </c>
       <c r="B127" t="s">
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="C127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C128">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>140</v>
       </c>
       <c r="B129" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C130">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>140</v>
-      </c>
-      <c r="B131" t="s">
-        <v>152</v>
-      </c>
-      <c r="C131">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>140</v>
-      </c>
-      <c r="B132" t="s">
-        <v>88</v>
-      </c>
-      <c r="C132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>140</v>
-      </c>
-      <c r="B133" t="s">
-        <v>89</v>
-      </c>
-      <c r="C133">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>140</v>
-      </c>
-      <c r="B134" t="s">
-        <v>50</v>
-      </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>140</v>
-      </c>
-      <c r="B135" t="s">
-        <v>52</v>
-      </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>140</v>
-      </c>
-      <c r="B136" t="s">
-        <v>53</v>
-      </c>
-      <c r="C136">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>140</v>
-      </c>
-      <c r="B137" t="s">
-        <v>55</v>
-      </c>
-      <c r="C137">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>140</v>
-      </c>
-      <c r="B138" t="s">
-        <v>166</v>
-      </c>
-      <c r="C138">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>140</v>
-      </c>
-      <c r="B139" t="s">
-        <v>61</v>
-      </c>
-      <c r="C139" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>140</v>
-      </c>
-      <c r="B140" t="s">
-        <v>65</v>
-      </c>
-      <c r="C140">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>140</v>
-      </c>
-      <c r="B141" t="s">
-        <v>159</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>140</v>
-      </c>
-      <c r="B142" t="s">
-        <v>75</v>
-      </c>
-      <c r="C142">
         <v>3</v>
       </c>
     </row>
@@ -5789,7 +5812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FB07A0-9E6E-4B88-B90E-57F2CD34A6BF}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -5797,13 +5820,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -5817,7 +5840,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -5831,7 +5854,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -5845,7 +5868,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -5859,7 +5882,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -5873,7 +5896,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -5887,7 +5910,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -5901,7 +5924,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -5915,7 +5938,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
start mmi tutorial, update data
</commit_message>
<xml_diff>
--- a/data/MMI_HW_data.xlsx
+++ b/data/MMI_HW_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_folder\R_projects_local\ENVS337\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfpom\Documents\ENVS337\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843EB7DC-9D38-4008-8837-621ED909A4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068D2F0-5847-4AF1-BA30-C4340602B067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8860" yWindow="970" windowWidth="10370" windowHeight="7350" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A75CC" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="172">
   <si>
     <t>Class</t>
   </si>
@@ -424,12 +424,6 @@
     <t>Platyhelminthes</t>
   </si>
   <si>
-    <t>Biotype1_sensitive</t>
-  </si>
-  <si>
-    <t>biotype1_tolerant</t>
-  </si>
-  <si>
     <t>Philopotamidae</t>
   </si>
   <si>
@@ -542,6 +536,24 @@
   </si>
   <si>
     <t>Polypedilum</t>
+  </si>
+  <si>
+    <t>sensitive_taxa</t>
+  </si>
+  <si>
+    <t>tolerant_taxa</t>
+  </si>
+  <si>
+    <t>pairwise</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB002BF-9427-4F54-99EB-0A769A51BC2F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -1432,7 +1444,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1443,7 +1455,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
@@ -1454,7 +1466,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -1465,7 +1477,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>87</v>
@@ -1476,7 +1488,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -1487,7 +1499,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
@@ -1498,7 +1510,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
         <v>88</v>
@@ -1509,7 +1521,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
         <v>89</v>
@@ -1520,7 +1532,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -1531,7 +1543,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
@@ -1542,7 +1554,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>91</v>
@@ -1553,7 +1565,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
@@ -1571,20 +1583,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1615,15 +1627,15 @@
         <v>107</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>125</v>
@@ -1632,22 +1644,22 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="b">
         <v>0</v>
@@ -1655,7 +1667,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>125</v>
@@ -1664,17 +1676,19 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>0</v>
@@ -1685,7 +1699,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>125</v>
@@ -1694,19 +1708,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>0</v>
@@ -1741,7 +1755,7 @@
         <v>109</v>
       </c>
       <c r="I5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1" t="b">
         <v>0</v>
@@ -1749,7 +1763,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>125</v>
@@ -1758,51 +1772,51 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>0</v>
@@ -1813,7 +1827,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>125</v>
@@ -1825,16 +1839,16 @@
         <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
@@ -1845,7 +1859,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>125</v>
@@ -1860,7 +1874,7 @@
         <v>49</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>116</v>
@@ -1877,7 +1891,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>125</v>
@@ -1892,7 +1906,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>116</v>
@@ -1909,7 +1923,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>164</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>125</v>
@@ -1923,9 +1937,7 @@
       <c r="E11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="1" t="s">
         <v>116</v>
       </c>
@@ -1940,8 +1952,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>52</v>
+      <c r="A12" t="s">
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>125</v>
@@ -1955,8 +1967,8 @@
       <c r="E12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>151</v>
+      <c r="F12" t="s">
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>116</v>
@@ -1973,7 +1985,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>125</v>
@@ -1988,7 +2000,7 @@
         <v>49</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>116</v>
@@ -2005,7 +2017,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>125</v>
@@ -2020,7 +2032,7 @@
         <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>116</v>
@@ -2029,7 +2041,7 @@
         <v>113</v>
       </c>
       <c r="I14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="b">
         <v>0</v>
@@ -2037,7 +2049,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>125</v>
@@ -2052,7 +2064,7 @@
         <v>49</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>116</v>
@@ -2069,7 +2081,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>125</v>
@@ -2084,7 +2096,7 @@
         <v>49</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>116</v>
@@ -2101,7 +2113,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>162</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>125</v>
@@ -2116,7 +2128,7 @@
         <v>49</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>116</v>
@@ -2133,7 +2145,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>125</v>
@@ -2148,13 +2160,13 @@
         <v>49</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>58</v>
+        <v>149</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
@@ -2165,7 +2177,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>125</v>
@@ -2180,7 +2192,7 @@
         <v>49</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>116</v>
@@ -2197,7 +2209,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>166</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>125</v>
@@ -2212,7 +2224,7 @@
         <v>49</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>116</v>
@@ -2229,7 +2241,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>125</v>
@@ -2244,7 +2256,7 @@
         <v>49</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>116</v>
@@ -2261,7 +2273,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>125</v>
@@ -2276,7 +2288,7 @@
         <v>49</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>116</v>
@@ -2293,7 +2305,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>125</v>
@@ -2308,7 +2320,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>116</v>
@@ -2325,7 +2337,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>125</v>
@@ -2337,16 +2349,16 @@
         <v>44</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>0</v>
@@ -2357,7 +2369,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>125</v>
@@ -2372,7 +2384,7 @@
         <v>49</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>116</v>
@@ -2389,7 +2401,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>125</v>
@@ -2403,7 +2415,9 @@
       <c r="E26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>116</v>
       </c>
@@ -2419,7 +2433,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>125</v>
@@ -2431,16 +2445,16 @@
         <v>44</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>0</v>
@@ -2451,7 +2465,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>125</v>
@@ -2460,22 +2474,20 @@
         <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>111</v>
       </c>
       <c r="I28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="1" t="b">
         <v>0</v>
@@ -2483,7 +2495,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>125</v>
@@ -2492,22 +2504,22 @@
         <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>111</v>
       </c>
       <c r="I29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="b">
         <v>0</v>
@@ -2515,7 +2527,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>125</v>
@@ -2524,20 +2536,22 @@
         <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G30" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>111</v>
       </c>
       <c r="I30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="1" t="b">
         <v>0</v>
@@ -2545,7 +2559,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>125</v>
@@ -2554,19 +2568,19 @@
         <v>5</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
@@ -2577,7 +2591,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>125</v>
@@ -2586,22 +2600,20 @@
         <v>5</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>86</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="1" t="b">
         <v>0</v>
@@ -2609,7 +2621,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>125</v>
@@ -2618,20 +2630,22 @@
         <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="1" t="b">
         <v>0</v>
@@ -2639,7 +2653,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>125</v>
@@ -2651,16 +2665,16 @@
         <v>44</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
@@ -2671,7 +2685,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>125</v>
@@ -2683,13 +2697,13 @@
         <v>44</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>111</v>
@@ -2703,7 +2717,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>125</v>
@@ -2715,11 +2729,11 @@
         <v>44</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>111</v>
@@ -2733,7 +2747,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>125</v>
@@ -2742,22 +2756,22 @@
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I37" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="1" t="b">
         <v>0</v>
@@ -2765,7 +2779,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>125</v>
@@ -2774,19 +2788,19 @@
         <v>5</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>0</v>
@@ -2821,7 +2835,7 @@
         <v>109</v>
       </c>
       <c r="I39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="1" t="b">
         <v>0</v>
@@ -2829,7 +2843,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>125</v>
@@ -2853,7 +2867,7 @@
         <v>109</v>
       </c>
       <c r="I40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="1" t="b">
         <v>0</v>
@@ -2861,7 +2875,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>125</v>
@@ -2885,7 +2899,7 @@
         <v>109</v>
       </c>
       <c r="I41" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="1" t="b">
         <v>0</v>
@@ -2917,7 +2931,7 @@
         <v>109</v>
       </c>
       <c r="I42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="1" t="b">
         <v>0</v>
@@ -2949,36 +2963,36 @@
         <v>113</v>
       </c>
       <c r="I43" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>16</v>
+      <c r="A44" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>16</v>
+        <v>70</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
@@ -2989,7 +3003,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>125</v>
@@ -3004,7 +3018,7 @@
         <v>15</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>108</v>
@@ -3013,7 +3027,7 @@
         <v>109</v>
       </c>
       <c r="I45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="1" t="b">
         <v>0</v>
@@ -3021,7 +3035,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>125</v>
@@ -3036,7 +3050,7 @@
         <v>15</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>108</v>
@@ -3045,7 +3059,7 @@
         <v>109</v>
       </c>
       <c r="I46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="1" t="b">
         <v>0</v>
@@ -3075,15 +3089,15 @@
         <v>109</v>
       </c>
       <c r="I47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
-        <v>93</v>
+      <c r="A48" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>125</v>
@@ -3094,20 +3108,20 @@
       <c r="D48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>93</v>
+      <c r="E48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="1" t="b">
         <v>0</v>
@@ -3115,7 +3129,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>125</v>
@@ -3124,20 +3138,14 @@
         <v>5</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>117</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
       <c r="I49" s="1" t="b">
         <v>0</v>
       </c>
@@ -3147,7 +3155,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>125</v>
@@ -3156,22 +3164,16 @@
         <v>5</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" s="1" t="b">
         <v>0</v>
@@ -3179,7 +3181,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>125</v>
@@ -3188,20 +3190,14 @@
         <v>5</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
@@ -3211,7 +3207,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>125</v>
@@ -3220,18 +3216,14 @@
         <v>5</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
       <c r="I52" s="1" t="b">
         <v>0</v>
       </c>
@@ -3241,7 +3233,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>125</v>
@@ -3250,19 +3242,17 @@
         <v>5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F53" s="4"/>
       <c r="G53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>0</v>
@@ -3273,31 +3263,31 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I54" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" s="1" t="b">
         <v>0</v>
@@ -3305,29 +3295,31 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F55" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="G55" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I55" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" s="1" t="b">
         <v>0</v>
@@ -3335,7 +3327,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>125</v>
@@ -3344,20 +3336,22 @@
         <v>5</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F56" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G56" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>115</v>
       </c>
       <c r="I56" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" s="1" t="b">
         <v>0</v>
@@ -3365,7 +3359,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>125</v>
@@ -3374,19 +3368,19 @@
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I57" s="1" t="b">
         <v>0</v>
@@ -3397,7 +3391,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>125</v>
@@ -3406,22 +3400,16 @@
         <v>5</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
       <c r="I58" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" s="1" t="b">
         <v>0</v>
@@ -3429,7 +3417,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>125</v>
@@ -3441,16 +3429,14 @@
         <v>19</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I59" s="1" t="b">
         <v>1</v>
@@ -3461,7 +3447,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>125</v>
@@ -3473,16 +3459,14 @@
         <v>19</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F60" s="4"/>
       <c r="G60" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I60" s="1" t="b">
         <v>1</v>
@@ -3493,7 +3477,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>125</v>
@@ -3505,14 +3489,16 @@
         <v>19</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F61" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="G61" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I61" s="1" t="b">
         <v>1</v>
@@ -3523,7 +3509,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>125</v>
@@ -3535,16 +3521,16 @@
         <v>19</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I62" s="1" t="b">
         <v>1</v>
@@ -3555,7 +3541,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>125</v>
@@ -3567,19 +3553,19 @@
         <v>19</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I63" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="1" t="b">
         <v>0</v>
@@ -3587,7 +3573,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>125</v>
@@ -3596,19 +3582,19 @@
         <v>5</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I64" s="1" t="b">
         <v>1</v>
@@ -3619,7 +3605,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>125</v>
@@ -3628,14 +3614,18 @@
         <v>5</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F65" s="4"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="G65" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I65" s="1" t="b">
         <v>1</v>
       </c>
@@ -3645,7 +3635,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>125</v>
@@ -3654,14 +3644,20 @@
         <v>5</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I66" s="1" t="b">
         <v>1</v>
       </c>
@@ -3671,7 +3667,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>125</v>
@@ -3683,13 +3679,13 @@
         <v>33</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" s="1" t="b">
         <v>0</v>
@@ -3697,25 +3693,29 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C68" s="4"/>
       <c r="D68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F68" s="4"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="I68" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" s="1" t="b">
         <v>0</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>125</v>
@@ -3732,17 +3732,19 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F69" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I69" s="1" t="b">
         <v>0</v>
@@ -3753,7 +3755,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>125</v>
@@ -3765,16 +3767,16 @@
         <v>33</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I70" s="1" t="b">
         <v>1</v>
@@ -3785,7 +3787,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>125</v>
@@ -3797,11 +3799,17 @@
         <v>33</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I71" s="1" t="b">
         <v>1</v>
       </c>
@@ -3811,7 +3819,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>125</v>
@@ -3823,11 +3831,17 @@
         <v>33</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I72" s="1" t="b">
         <v>1</v>
       </c>
@@ -3837,7 +3851,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>125</v>
@@ -3869,7 +3883,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>163</v>
+        <v>84</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>125</v>
@@ -3901,7 +3915,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>125</v>
@@ -3933,7 +3947,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>125</v>
@@ -3965,7 +3979,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>125</v>
@@ -3974,22 +3988,22 @@
         <v>5</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I77" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77" s="1" t="b">
         <v>0</v>
@@ -3997,7 +4011,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>125</v>
@@ -4006,22 +4020,20 @@
         <v>5</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>119</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F78" s="4"/>
       <c r="G78" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I78" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J78" s="1" t="b">
         <v>0</v>
@@ -4029,7 +4041,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>125</v>
@@ -4038,22 +4050,22 @@
         <v>5</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I79" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" s="1" t="b">
         <v>0</v>
@@ -4061,7 +4073,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>125</v>
@@ -4073,10 +4085,10 @@
         <v>70</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>117</v>
@@ -4093,28 +4105,28 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I81" s="1" t="b">
         <v>0</v>
@@ -4125,28 +4137,28 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I82" s="1" t="b">
         <v>0</v>
@@ -4157,28 +4169,28 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I83" s="1" t="b">
         <v>0</v>
@@ -4189,28 +4201,26 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>104</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="F84" s="4"/>
       <c r="G84" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I84" s="1" t="b">
         <v>0</v>
@@ -4221,15 +4231,23 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>117</v>
       </c>
@@ -4245,22 +4263,20 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>75</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="5"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I86" s="1" t="b">
         <v>0</v>
@@ -4271,22 +4287,22 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="5"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I87" s="1" t="b">
         <v>0</v>
@@ -4297,13 +4313,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="5"/>
@@ -4323,21 +4339,17 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>162</v>
+        <v>77</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>162</v>
-      </c>
+      <c r="C89" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
         <v>117</v>
       </c>
@@ -4352,11 +4364,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J88">
-    <sortCondition ref="D2:D88"/>
-    <sortCondition ref="E2:E88"/>
-    <sortCondition ref="F2:F88"/>
-    <sortCondition ref="A2:A88"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J89">
+    <sortCondition ref="E2:E89"/>
+    <sortCondition ref="A2:A89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4389,7 +4399,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -4400,7 +4410,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -4411,7 +4421,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -4422,7 +4432,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -4433,7 +4443,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -4444,7 +4454,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -4455,7 +4465,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -4466,7 +4476,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -4477,7 +4487,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
         <v>80</v>
@@ -4488,7 +4498,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -4499,7 +4509,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -4510,7 +4520,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>82</v>
@@ -4521,7 +4531,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
         <v>83</v>
@@ -4532,7 +4542,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
@@ -4543,7 +4553,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
@@ -4554,7 +4564,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
         <v>50</v>
@@ -4565,7 +4575,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
@@ -4576,7 +4586,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
@@ -4587,7 +4597,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>58</v>
@@ -4598,7 +4608,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
@@ -4609,7 +4619,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
@@ -4620,7 +4630,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>86</v>
@@ -4631,7 +4641,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
@@ -4642,7 +4652,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
@@ -4653,7 +4663,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
@@ -4664,7 +4674,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
         <v>78</v>
@@ -4675,7 +4685,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4686,7 +4696,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
@@ -4697,7 +4707,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -4708,7 +4718,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -4719,7 +4729,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
@@ -4730,7 +4740,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -4741,7 +4751,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
         <v>79</v>
@@ -4752,7 +4762,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
@@ -4763,7 +4773,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -4774,7 +4784,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
         <v>84</v>
@@ -4785,10 +4795,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -4796,7 +4806,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
         <v>48</v>
@@ -4807,7 +4817,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>50</v>
@@ -4818,7 +4828,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
         <v>86</v>
@@ -4829,10 +4839,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -4840,7 +4850,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
         <v>72</v>
@@ -4851,7 +4861,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
         <v>74</v>
@@ -4862,7 +4872,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
         <v>77</v>
@@ -4873,7 +4883,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -4884,10 +4894,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -4895,7 +4905,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -4906,7 +4916,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -4917,7 +4927,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -4928,7 +4938,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
@@ -4939,7 +4949,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -4950,10 +4960,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -4961,7 +4971,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
         <v>79</v>
@@ -4972,7 +4982,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
@@ -4983,7 +4993,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
         <v>87</v>
@@ -4994,7 +5004,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
         <v>83</v>
@@ -5005,10 +5015,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -5016,7 +5026,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
@@ -5027,7 +5037,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B60" t="s">
         <v>50</v>
@@ -5038,10 +5048,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -5049,7 +5059,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B62" t="s">
         <v>56</v>
@@ -5060,7 +5070,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
@@ -5071,10 +5081,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -5082,7 +5092,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
         <v>72</v>
@@ -5093,10 +5103,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -5104,7 +5114,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -5115,7 +5125,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
@@ -5126,7 +5136,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
         <v>25</v>
@@ -5137,7 +5147,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" t="s">
         <v>79</v>
@@ -5148,7 +5158,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
         <v>32</v>
@@ -5159,7 +5169,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B72" t="s">
         <v>35</v>
@@ -5170,7 +5180,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" t="s">
         <v>37</v>
@@ -5181,10 +5191,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -5192,7 +5202,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
         <v>84</v>
@@ -5203,7 +5213,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B76" t="s">
         <v>46</v>
@@ -5214,7 +5224,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
         <v>48</v>
@@ -5225,7 +5235,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B78" t="s">
         <v>89</v>
@@ -5236,7 +5246,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
         <v>50</v>
@@ -5247,7 +5257,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
@@ -5258,7 +5268,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B81" t="s">
         <v>55</v>
@@ -5269,7 +5279,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
         <v>86</v>
@@ -5280,7 +5290,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B83" t="s">
         <v>72</v>
@@ -5291,7 +5301,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
         <v>74</v>
@@ -5302,7 +5312,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s">
         <v>77</v>
@@ -5313,7 +5323,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s">
         <v>10</v>
@@ -5324,7 +5334,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B87" t="s">
         <v>12</v>
@@ -5335,7 +5345,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
         <v>18</v>
@@ -5346,7 +5356,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
         <v>21</v>
@@ -5357,10 +5367,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -5368,7 +5378,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
         <v>79</v>
@@ -5379,7 +5389,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B92" t="s">
         <v>27</v>
@@ -5390,7 +5400,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
         <v>32</v>
@@ -5401,7 +5411,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
         <v>37</v>
@@ -5412,7 +5422,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B95" t="s">
         <v>46</v>
@@ -5423,7 +5433,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B96" t="s">
         <v>88</v>
@@ -5434,7 +5444,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B97" t="s">
         <v>89</v>
@@ -5445,7 +5455,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B98" t="s">
         <v>50</v>
@@ -5456,10 +5466,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B99" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C99">
         <v>4</v>
@@ -5467,7 +5477,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B100" t="s">
         <v>53</v>
@@ -5478,7 +5488,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B101" t="s">
         <v>62</v>
@@ -5489,7 +5499,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B102" t="s">
         <v>86</v>
@@ -5500,7 +5510,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
         <v>72</v>
@@ -5511,7 +5521,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B104" t="s">
         <v>74</v>
@@ -5522,7 +5532,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
@@ -5533,7 +5543,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
@@ -5544,7 +5554,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B107" t="s">
         <v>18</v>
@@ -5555,7 +5565,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
         <v>23</v>
@@ -5566,7 +5576,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
         <v>79</v>
@@ -5577,7 +5587,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B110" t="s">
         <v>29</v>
@@ -5588,7 +5598,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
         <v>80</v>
@@ -5599,7 +5609,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B112" t="s">
         <v>28</v>
@@ -5610,7 +5620,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B113" t="s">
         <v>32</v>
@@ -5621,7 +5631,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B114" t="s">
         <v>37</v>
@@ -5632,10 +5642,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B115" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -5643,7 +5653,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B116" t="s">
         <v>83</v>
@@ -5654,7 +5664,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B117" t="s">
         <v>84</v>
@@ -5665,7 +5675,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
         <v>40</v>
@@ -5676,10 +5686,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B119" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C119">
         <v>2</v>
@@ -5687,7 +5697,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B120" t="s">
         <v>88</v>
@@ -5698,7 +5708,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
         <v>89</v>
@@ -5709,7 +5719,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
         <v>50</v>
@@ -5720,7 +5730,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
         <v>52</v>
@@ -5731,7 +5741,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
         <v>53</v>
@@ -5742,7 +5752,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
         <v>55</v>
@@ -5753,10 +5763,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C126">
         <v>7</v>
@@ -5764,7 +5774,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B127" t="s">
         <v>61</v>
@@ -5775,7 +5785,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B128" t="s">
         <v>65</v>
@@ -5786,10 +5796,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B129" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -5797,7 +5807,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B130" t="s">
         <v>75</v>
@@ -5814,19 +5824,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FB07A0-9E6E-4B88-B90E-57F2CD34A6BF}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -5834,111 +5845,126 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>142</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>135</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>143</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>136</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>137</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>145</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>138</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>146</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>148</v>
-      </c>
       <c r="C8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="E8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -5946,10 +5972,10 @@
         <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" t="s">
-        <v>132</v>
+        <v>171</v>
+      </c>
+      <c r="E9" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mmi tutorial and hw key
</commit_message>
<xml_diff>
--- a/data/MMI_HW_data.xlsx
+++ b/data/MMI_HW_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfpom\Documents\ENVS337\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_folder\R_projects_local\ENVS337\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068D2F0-5847-4AF1-BA30-C4340602B067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8507D916-DCC3-428B-A524-05310B046928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="970" windowWidth="10370" windowHeight="7350" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A75CC" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="172">
   <si>
     <t>Class</t>
   </si>
@@ -541,19 +541,19 @@
     <t>sensitive_taxa</t>
   </si>
   <si>
-    <t>tolerant_taxa</t>
-  </si>
-  <si>
     <t>pairwise</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>Animas_upper</t>
+  </si>
+  <si>
+    <t>Elk_Cr</t>
+  </si>
+  <si>
+    <t>Cascade_Cr</t>
+  </si>
+  <si>
+    <t>Bio2_sensitive</t>
   </si>
 </sst>
 </file>
@@ -914,14 +914,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
@@ -954,7 +954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -965,7 +965,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -976,7 +976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>122</v>
       </c>
@@ -998,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>122</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>122</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>122</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>122</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>122</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>122</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>122</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>122</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>122</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>122</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>122</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>122</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>122</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>122</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>122</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>122</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>122</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>122</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>122</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>122</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>122</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>122</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>122</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>122</v>
       </c>
@@ -1429,9 +1429,9 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1583,25 +1583,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="B43" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1630,10 +1630,10 @@
         <v>166</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1662,10 +1662,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>97</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>88</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>89</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>51</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>157</v>
       </c>
@@ -2044,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>156</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>162</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>90</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>91</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>59</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>164</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -2490,10 +2490,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>154</v>
       </c>
@@ -2522,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -2554,10 +2554,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>100</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
@@ -2616,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
@@ -2648,10 +2648,10 @@
         <v>1</v>
       </c>
       <c r="J33" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>85</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>61</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>60</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>63</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>118</v>
       </c>
@@ -2838,10 +2838,10 @@
         <v>1</v>
       </c>
       <c r="J39" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>153</v>
       </c>
@@ -2870,10 +2870,10 @@
         <v>1</v>
       </c>
       <c r="J40" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>12</v>
       </c>
@@ -2902,10 +2902,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
@@ -2934,10 +2934,10 @@
         <v>1</v>
       </c>
       <c r="J42" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>14</v>
       </c>
@@ -2966,10 +2966,10 @@
         <v>1</v>
       </c>
       <c r="J43" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>152</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -3030,10 +3030,10 @@
         <v>1</v>
       </c>
       <c r="J45" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>17</v>
       </c>
@@ -3062,10 +3062,10 @@
         <v>1</v>
       </c>
       <c r="J46" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>15</v>
       </c>
@@ -3092,10 +3092,10 @@
         <v>1</v>
       </c>
       <c r="J47" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
@@ -3124,10 +3124,10 @@
         <v>1</v>
       </c>
       <c r="J48" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>37</v>
       </c>
@@ -3144,8 +3144,12 @@
         <v>36</v>
       </c>
       <c r="F49" s="4"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I49" s="1" t="b">
         <v>0</v>
       </c>
@@ -3153,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>87</v>
       </c>
@@ -3170,8 +3174,12 @@
         <v>36</v>
       </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I50" s="1" t="b">
         <v>0</v>
       </c>
@@ -3179,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>147</v>
       </c>
@@ -3196,8 +3204,12 @@
         <v>36</v>
       </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="G51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>38</v>
       </c>
@@ -3222,8 +3234,12 @@
         <v>36</v>
       </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I52" s="1" t="b">
         <v>0</v>
       </c>
@@ -3231,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>36</v>
       </c>
@@ -3261,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>102</v>
       </c>
@@ -3293,7 +3309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>72</v>
       </c>
@@ -3325,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -3351,13 +3367,13 @@
         <v>115</v>
       </c>
       <c r="I56" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>93</v>
       </c>
@@ -3389,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>163</v>
       </c>
@@ -3406,8 +3422,12 @@
         <v>163</v>
       </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
       </c>
@@ -3415,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>24</v>
       </c>
@@ -3442,10 +3462,10 @@
         <v>1</v>
       </c>
       <c r="J59" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>25</v>
       </c>
@@ -3472,10 +3492,10 @@
         <v>1</v>
       </c>
       <c r="J60" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>79</v>
       </c>
@@ -3504,10 +3524,10 @@
         <v>1</v>
       </c>
       <c r="J61" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>27</v>
       </c>
@@ -3536,10 +3556,10 @@
         <v>1</v>
       </c>
       <c r="J62" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>29</v>
       </c>
@@ -3568,10 +3588,10 @@
         <v>1</v>
       </c>
       <c r="J63" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>80</v>
       </c>
@@ -3600,10 +3620,10 @@
         <v>1</v>
       </c>
       <c r="J64" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>28</v>
       </c>
@@ -3630,10 +3650,10 @@
         <v>1</v>
       </c>
       <c r="J65" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>30</v>
       </c>
@@ -3662,10 +3682,10 @@
         <v>1</v>
       </c>
       <c r="J66" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>128</v>
       </c>
@@ -3682,8 +3702,12 @@
         <v>128</v>
       </c>
       <c r="F67" s="4"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
+      <c r="G67" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I67" s="1" t="b">
         <v>0</v>
       </c>
@@ -3691,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>160</v>
       </c>
@@ -3721,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>95</v>
       </c>
@@ -3747,13 +3771,13 @@
         <v>115</v>
       </c>
       <c r="I69" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>119</v>
       </c>
@@ -3782,10 +3806,10 @@
         <v>1</v>
       </c>
       <c r="J70" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>161</v>
       </c>
@@ -3814,10 +3838,10 @@
         <v>1</v>
       </c>
       <c r="J71" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>83</v>
       </c>
@@ -3846,10 +3870,10 @@
         <v>1</v>
       </c>
       <c r="J72" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>155</v>
       </c>
@@ -3878,10 +3902,10 @@
         <v>1</v>
       </c>
       <c r="J73" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>84</v>
       </c>
@@ -3910,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="J74" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>40</v>
       </c>
@@ -3942,10 +3966,10 @@
         <v>1</v>
       </c>
       <c r="J75" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>150</v>
       </c>
@@ -3974,10 +3998,10 @@
         <v>1</v>
       </c>
       <c r="J76" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>65</v>
       </c>
@@ -4009,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>64</v>
       </c>
@@ -4039,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>86</v>
       </c>
@@ -4071,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>74</v>
       </c>
@@ -4103,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>32</v>
       </c>
@@ -4135,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>67</v>
       </c>
@@ -4167,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>68</v>
       </c>
@@ -4199,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>66</v>
       </c>
@@ -4229,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>104</v>
       </c>
@@ -4261,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>78</v>
       </c>
@@ -4285,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>75</v>
       </c>
@@ -4311,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>76</v>
       </c>
@@ -4337,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>77</v>
       </c>
@@ -4381,12 +4405,12 @@
       <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -4397,7 +4421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -4408,7 +4432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -4419,7 +4443,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -4430,7 +4454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -4441,7 +4465,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -4452,7 +4476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -4463,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -4474,7 +4498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -4485,7 +4509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -4496,7 +4520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -4507,7 +4531,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -4518,7 +4542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -4529,7 +4553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -4540,7 +4564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -4551,7 +4575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>132</v>
       </c>
@@ -4562,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>132</v>
       </c>
@@ -4573,7 +4597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -4584,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -4595,7 +4619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4606,7 +4630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -4617,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -4628,7 +4652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -4639,7 +4663,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -4650,7 +4674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4661,7 +4685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -4672,7 +4696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -4683,7 +4707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -4694,7 +4718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -4705,7 +4729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -4716,7 +4740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -4727,7 +4751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -4738,7 +4762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -4749,7 +4773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -4760,7 +4784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -4771,7 +4795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -4782,7 +4806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -4793,7 +4817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -4804,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -4815,7 +4839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -4826,7 +4850,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -4837,7 +4861,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -4848,7 +4872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>133</v>
       </c>
@@ -4859,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -4870,7 +4894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -4881,7 +4905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -4892,7 +4916,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>134</v>
       </c>
@@ -4903,7 +4927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>134</v>
       </c>
@@ -4914,7 +4938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>134</v>
       </c>
@@ -4925,7 +4949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -4936,7 +4960,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -4947,7 +4971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>134</v>
       </c>
@@ -4958,7 +4982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -4969,7 +4993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>134</v>
       </c>
@@ -4980,7 +5004,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -4991,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -5002,7 +5026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -5013,7 +5037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>134</v>
       </c>
@@ -5024,7 +5048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -5035,7 +5059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -5046,7 +5070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>134</v>
       </c>
@@ -5057,7 +5081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>134</v>
       </c>
@@ -5068,7 +5092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -5079,7 +5103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>134</v>
       </c>
@@ -5090,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -5101,7 +5125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>134</v>
       </c>
@@ -5112,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -5123,7 +5147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -5134,7 +5158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -5145,7 +5169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -5156,7 +5180,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>136</v>
       </c>
@@ -5167,7 +5191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -5178,7 +5202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -5189,7 +5213,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>136</v>
       </c>
@@ -5200,7 +5224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -5211,7 +5235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>136</v>
       </c>
@@ -5222,7 +5246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -5233,7 +5257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>136</v>
       </c>
@@ -5244,7 +5268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>136</v>
       </c>
@@ -5255,7 +5279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>136</v>
       </c>
@@ -5266,7 +5290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>136</v>
       </c>
@@ -5277,7 +5301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -5288,7 +5312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>136</v>
       </c>
@@ -5299,7 +5323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>136</v>
       </c>
@@ -5310,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>136</v>
       </c>
@@ -5321,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>137</v>
       </c>
@@ -5332,7 +5356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>137</v>
       </c>
@@ -5343,7 +5367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>137</v>
       </c>
@@ -5354,7 +5378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>137</v>
       </c>
@@ -5365,7 +5389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>137</v>
       </c>
@@ -5376,7 +5400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -5387,7 +5411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>137</v>
       </c>
@@ -5398,7 +5422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>137</v>
       </c>
@@ -5409,7 +5433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>137</v>
       </c>
@@ -5420,7 +5444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>137</v>
       </c>
@@ -5431,7 +5455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>137</v>
       </c>
@@ -5442,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -5453,7 +5477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>137</v>
       </c>
@@ -5464,7 +5488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>137</v>
       </c>
@@ -5475,7 +5499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>137</v>
       </c>
@@ -5486,7 +5510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>137</v>
       </c>
@@ -5497,7 +5521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>137</v>
       </c>
@@ -5508,7 +5532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>137</v>
       </c>
@@ -5519,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>137</v>
       </c>
@@ -5530,7 +5554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>138</v>
       </c>
@@ -5541,7 +5565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -5552,7 +5576,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>138</v>
       </c>
@@ -5563,7 +5587,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>138</v>
       </c>
@@ -5574,7 +5598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>138</v>
       </c>
@@ -5585,7 +5609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>138</v>
       </c>
@@ -5596,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>138</v>
       </c>
@@ -5607,7 +5631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>138</v>
       </c>
@@ -5618,7 +5642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>138</v>
       </c>
@@ -5629,7 +5653,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>138</v>
       </c>
@@ -5640,7 +5664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>138</v>
       </c>
@@ -5651,7 +5675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>138</v>
       </c>
@@ -5662,7 +5686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>138</v>
       </c>
@@ -5673,7 +5697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>138</v>
       </c>
@@ -5684,7 +5708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -5695,7 +5719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>138</v>
       </c>
@@ -5706,7 +5730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -5717,7 +5741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -5728,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -5739,7 +5763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -5750,7 +5774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>138</v>
       </c>
@@ -5761,7 +5785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -5772,7 +5796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -5783,7 +5807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>138</v>
       </c>
@@ -5794,7 +5818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -5805,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>138</v>
       </c>
@@ -5827,17 +5851,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -5845,7 +5869,7 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
         <v>131</v>
@@ -5854,7 +5878,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -5868,7 +5892,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -5882,7 +5906,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -5890,7 +5914,7 @@
         <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -5899,7 +5923,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -5907,7 +5931,7 @@
         <v>143</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -5916,7 +5940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -5924,7 +5948,7 @@
         <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -5933,7 +5957,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -5941,7 +5965,7 @@
         <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -5950,7 +5974,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -5958,13 +5982,13 @@
         <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -5972,7 +5996,7 @@
         <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9" t="s">
         <v>130</v>

</xml_diff>